<commit_message>
Adicionadas escolhas da versão do algoritmo e tamanho da chave
</commit_message>
<xml_diff>
--- a/src/main/resources/report.xlsx
+++ b/src/main/resources/report.xlsx
@@ -23,13 +23,13 @@
     <t>SHA256withECDSA</t>
   </si>
   <si>
-    <t>Dilithium5</t>
-  </si>
-  <si>
-    <t>Falcon-1024</t>
-  </si>
-  <si>
-    <t>SPHINCS+-SHAKE-256s-simple</t>
+    <t>Dilithium2</t>
+  </si>
+  <si>
+    <t>Falcon-512</t>
+  </si>
+  <si>
+    <t>SPHINCS+-SHA2-128f-simple</t>
   </si>
   <si>
     <t>isPostQuantum</t>
@@ -234,19 +234,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n" s="2">
-        <v>256.0</v>
+        <v>128.0</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>70.0</v>
+        <v>72.0</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>4595.0</v>
+        <v>2420.0</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>1273.0</v>
+        <v>654.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>29792.0</v>
+        <v>17088.0</v>
       </c>
     </row>
     <row r="5">
@@ -254,19 +254,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="n" s="2">
-        <v>294.0</v>
+        <v>162.0</v>
       </c>
       <c r="C5" t="n" s="2">
         <v>91.0</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>2592.0</v>
+        <v>1312.0</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>1793.0</v>
+        <v>897.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>64.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="6">
@@ -274,19 +274,19 @@
         <v>12</v>
       </c>
       <c r="B6" t="n" s="2">
-        <v>1217.0</v>
+        <v>635.0</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>67.0</v>
+        <v>150.0</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>4864.0</v>
+        <v>2528.0</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>2305.0</v>
+        <v>1281.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>128.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="7">
@@ -294,19 +294,19 @@
         <v>13</v>
       </c>
       <c r="B7" t="n" s="2">
-        <v>6.9612944E7</v>
+        <v>1.48186112E8</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>1534602.0</v>
+        <v>2178852.0</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>83507.0</v>
+        <v>35983.0</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>2.0701484E7</v>
+        <v>9695598.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>5.0214876E7</v>
+        <v>333133.0</v>
       </c>
     </row>
     <row r="8">
@@ -334,19 +334,19 @@
         <v>15</v>
       </c>
       <c r="B9" t="n" s="2">
-        <v>4427758.0</v>
+        <v>648755.0</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>1880494.0</v>
+        <v>2924291.0</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>148340.0</v>
+        <v>50663.0</v>
       </c>
       <c r="E9" t="n" s="2">
-        <v>655661.0</v>
+        <v>446189.0</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>5.985104E8</v>
+        <v>8258050.0</v>
       </c>
     </row>
     <row r="10">
@@ -374,19 +374,19 @@
         <v>17</v>
       </c>
       <c r="B11" t="n" s="2">
-        <v>133555.0</v>
+        <v>88476.0</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>3309742.0</v>
+        <v>4067236.0</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>81895.0</v>
+        <v>34141.0</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>126917.0</v>
+        <v>55766.0</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>1058517.0</v>
+        <v>847349.0</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
Geração de tabela mais bonita
</commit_message>
<xml_diff>
--- a/src/main/resources/report.xlsx
+++ b/src/main/resources/report.xlsx
@@ -32,7 +32,7 @@
     <t>SPHINCS+-SHA2-128f-simple</t>
   </si>
   <si>
-    <t>isPostQuantum</t>
+    <t>Is post-quantum?</t>
   </si>
   <si>
     <t>false</t>
@@ -41,34 +41,34 @@
     <t>true</t>
   </si>
   <si>
-    <t>executionTimes</t>
-  </si>
-  <si>
-    <t>signatureSize</t>
-  </si>
-  <si>
-    <t>publicKeySize</t>
-  </si>
-  <si>
-    <t>privateKeySize</t>
-  </si>
-  <si>
-    <t>keyGenTimeMean</t>
-  </si>
-  <si>
-    <t>keyGenTimeStandardDeviation</t>
-  </si>
-  <si>
-    <t>signatureTimeMean</t>
-  </si>
-  <si>
-    <t>signatureTimeStandardDeviation</t>
-  </si>
-  <si>
-    <t>verifyTimeMean</t>
-  </si>
-  <si>
-    <t>verifyTimeStandardDeviation</t>
+    <t>Execution times</t>
+  </si>
+  <si>
+    <t>Signature size (B)</t>
+  </si>
+  <si>
+    <t>Public key size (B)</t>
+  </si>
+  <si>
+    <t>Private key size (B)</t>
+  </si>
+  <si>
+    <t>Keys gen time mean (ns)</t>
+  </si>
+  <si>
+    <t>Keys gen time standard deviation (ns)</t>
+  </si>
+  <si>
+    <t>Signature time mean (ns)</t>
+  </si>
+  <si>
+    <t>Signature time standard deviation (ns)</t>
+  </si>
+  <si>
+    <t>Verify time mean (ns)</t>
+  </si>
+  <si>
+    <t>Verify time standard deviation (ns)</t>
   </si>
 </sst>
 </file>
@@ -76,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -88,6 +88,10 @@
       <name val="Arial"/>
       <sz val="14.0"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -98,12 +102,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="48"/>
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="48"/>
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,9 +143,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
+      <alignment wrapText="true" horizontal="right"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -169,27 +175,27 @@
     <col min="12" max="12" width="23.4375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="37.5" customHeight="true">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="37.5" customHeight="true">
       <c r="A2" t="s" s="1">
         <v>6</v>
       </c>
@@ -209,27 +215,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="37.5" customHeight="true">
       <c r="A3" t="s" s="1">
         <v>9</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>1.0</v>
+        <v>100.0</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>1.0</v>
+        <v>100.0</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>1.0</v>
+        <v>100.0</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>1.0</v>
+        <v>100.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="4" ht="37.5" customHeight="true">
       <c r="A4" t="s" s="1">
         <v>10</v>
       </c>
@@ -243,13 +249,13 @@
         <v>2420.0</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>656.0</v>
+        <v>655.0</v>
       </c>
       <c r="F4" t="n" s="2">
         <v>17088.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="37.5" customHeight="true">
       <c r="A5" t="s" s="1">
         <v>11</v>
       </c>
@@ -269,12 +275,12 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="37.5" customHeight="true">
       <c r="A6" t="s" s="1">
         <v>12</v>
       </c>
       <c r="B6" t="n" s="2">
-        <v>634.0</v>
+        <v>635.0</v>
       </c>
       <c r="C6" t="n" s="2">
         <v>150.0</v>
@@ -289,124 +295,124 @@
         <v>64.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="37.5" customHeight="true">
       <c r="A7" t="s" s="1">
         <v>13</v>
       </c>
       <c r="B7" t="n" s="2">
-        <v>3.4641176E7</v>
+        <v>2.8950392E7</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>2922764.0</v>
+        <v>968381.0</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>41780.0</v>
+        <v>39135.0</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>6487213.0</v>
+        <v>8997841.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>456347.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>420322.0</v>
+      </c>
+    </row>
+    <row r="8" ht="37.5" customHeight="true">
       <c r="A8" t="s" s="1">
         <v>14</v>
       </c>
       <c r="B8" t="n" s="2">
-        <v>0.0</v>
+        <v>1.6790592E7</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>0.0</v>
+        <v>144602.0</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>0.0</v>
+        <v>2864.0</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>0.0</v>
+        <v>1904224.0</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>25897.0</v>
+      </c>
+    </row>
+    <row r="9" ht="37.5" customHeight="true">
       <c r="A9" t="s" s="1">
         <v>15</v>
       </c>
       <c r="B9" t="n" s="2">
-        <v>761234.0</v>
+        <v>390125.0</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>6769271.0</v>
+        <v>575886.0</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>50875.0</v>
+        <v>94352.0</v>
       </c>
       <c r="E9" t="n" s="2">
-        <v>424425.0</v>
+        <v>367723.0</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>9404871.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>9761512.0</v>
+      </c>
+    </row>
+    <row r="10" ht="37.5" customHeight="true">
       <c r="A10" t="s" s="1">
         <v>16</v>
       </c>
       <c r="B10" t="n" s="2">
-        <v>0.0</v>
+        <v>70077.0</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>0.0</v>
+        <v>84300.0</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>0.0</v>
+        <v>50797.0</v>
       </c>
       <c r="E10" t="n" s="2">
-        <v>0.0</v>
+        <v>16987.0</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>341901.0</v>
+      </c>
+    </row>
+    <row r="11" ht="37.5" customHeight="true">
       <c r="A11" t="s" s="1">
         <v>17</v>
       </c>
       <c r="B11" t="n" s="2">
-        <v>90798.0</v>
+        <v>76659.0</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>6167630.0</v>
+        <v>1866386.0</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>30908.0</v>
+        <v>36509.0</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>66364.0</v>
+        <v>68632.0</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>954714.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>867417.0</v>
+      </c>
+    </row>
+    <row r="12" ht="37.5" customHeight="true">
       <c r="A12" t="s" s="1">
         <v>18</v>
       </c>
       <c r="B12" t="n" s="2">
-        <v>0.0</v>
+        <v>17937.0</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>0.0</v>
+        <v>153704.0</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>0.0</v>
+        <v>2443.0</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>0.0</v>
+        <v>2715.0</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>0.0</v>
+        <v>33777.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
liboqs-java adicionada ao pom
</commit_message>
<xml_diff>
--- a/src/main/resources/report.xlsx
+++ b/src/main/resources/report.xlsx
@@ -220,19 +220,19 @@
         <v>9</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4" ht="37.5" customHeight="true">
@@ -249,7 +249,7 @@
         <v>2420.0</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>655.0</v>
+        <v>656.0</v>
       </c>
       <c r="F4" t="n" s="2">
         <v>17088.0</v>
@@ -280,7 +280,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n" s="2">
-        <v>636.0</v>
+        <v>634.0</v>
       </c>
       <c r="C6" t="n" s="2">
         <v>150.0</v>
@@ -300,19 +300,19 @@
         <v>13</v>
       </c>
       <c r="B7" t="n" s="2">
-        <v>4.7245928E7</v>
+        <v>1.9704932E7</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>1681994.0</v>
+        <v>2079010.0</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>66798.0</v>
+        <v>64777.0</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>7294869.0</v>
+        <v>7923051.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>439387.0</v>
+        <v>353757.0</v>
       </c>
     </row>
     <row r="8" ht="37.5" customHeight="true">
@@ -320,19 +320,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="n" s="2">
-        <v>2.8594217E7</v>
+        <v>0.0</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>369628.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>13974.0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>1120789.0</v>
+        <v>0.0</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>36230.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" ht="37.5" customHeight="true">
@@ -340,19 +340,19 @@
         <v>15</v>
       </c>
       <c r="B9" t="n" s="2">
-        <v>535324.0</v>
+        <v>851071.0</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>2011883.0</v>
+        <v>3127962.0</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>139871.0</v>
+        <v>114526.0</v>
       </c>
       <c r="E9" t="n" s="2">
-        <v>287059.0</v>
+        <v>352860.0</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>9970009.0</v>
+        <v>8541412.0</v>
       </c>
     </row>
     <row r="10" ht="37.5" customHeight="true">
@@ -360,19 +360,19 @@
         <v>16</v>
       </c>
       <c r="B10" t="n" s="2">
-        <v>109632.0</v>
+        <v>0.0</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>682249.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>74968.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n" s="2">
-        <v>17918.0</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>288505.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" ht="37.5" customHeight="true">
@@ -380,19 +380,19 @@
         <v>17</v>
       </c>
       <c r="B11" t="n" s="2">
-        <v>77484.0</v>
+        <v>232219.0</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>3305299.0</v>
+        <v>6672071.0</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>38604.0</v>
+        <v>37758.0</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>56878.0</v>
+        <v>61203.0</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>876084.0</v>
+        <v>816434.0</v>
       </c>
     </row>
     <row r="12" ht="37.5" customHeight="true">
@@ -400,19 +400,19 @@
         <v>18</v>
       </c>
       <c r="B12" t="n" s="2">
-        <v>2300.0</v>
+        <v>0.0</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>1191201.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>8385.0</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>7487.0</v>
+        <v>0.0</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>22905.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>